<commit_message>
mejoras en usabilidad y verificacion de impresiones
</commit_message>
<xml_diff>
--- a/BULKAPP/app/TTD_ESC_file.xlsx
+++ b/BULKAPP/app/TTD_ESC_file.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="424">
   <si>
     <t>Name (required)</t>
   </si>
@@ -1127,7 +1127,7 @@
     <t>Weborama</t>
   </si>
   <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V1-DB_300x600</t>
+    <t>iese-eu_v1mp_DEG-MIM-DEMAND-GEN-DISPLAY-GOOGLE-ONLINE-PAID-24-25-EN_dis_prs-1_DB-V1_300x600</t>
   </si>
   <si>
     <t>300</t>
@@ -1136,25 +1136,25 @@
     <t>600</t>
   </si>
   <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v1/300x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v1-db&amp;utm_content=300x600&amp;tc_alt=140145" width="300" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140145&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/</t>
+    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/09/degree_online/300x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-mim/?utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=701Qu00000D9OyE&amp;utm_term=prs-db-version1&amp;utm_content=300x600&amp;tc_alt=143236" width="300" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=143236&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>https://formscloud.iese.edu/landings-mim/</t>
   </si>
   <si>
     <t>yes</t>
   </si>
   <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V1-DB_300x250</t>
+    <t>iese-eu_v1mp_DEG-MIM-DEMAND-GEN-DISPLAY-GOOGLE-ONLINE-PAID-24-25-EN_dis_prs-1_DB-V1_300x250</t>
   </si>
   <si>
     <t>250</t>
   </si>
   <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v1/300x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v1-db&amp;utm_content=300x250&amp;tc_alt=140146" width="300" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140146&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V1-DB_320x100</t>
+    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/09/degree_online/300x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-mim/?utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=701Qu00000D9OyE&amp;utm_term=prs-db-version1&amp;utm_content=300x250&amp;tc_alt=143237" width="300" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=143237&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>iese-eu_v1mp_DEG-MIM-DEMAND-GEN-DISPLAY-GOOGLE-ONLINE-PAID-24-25-EN_dis_prs-1_DB-V1_320x100</t>
   </si>
   <si>
     <t>320</t>
@@ -1163,28 +1163,28 @@
     <t>100</t>
   </si>
   <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v1/320x100/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v1-db&amp;utm_content=320x100&amp;tc_alt=140147" width="320" height="100" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140147&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V1-DB_970x250</t>
+    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/09/degree_online/320x100/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-mim/?utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=701Qu00000D9OyE&amp;utm_term=prs-db-version1&amp;utm_content=320x100&amp;tc_alt=143238" width="320" height="100" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=143238&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>iese-eu_v1mp_DEG-MIM-DEMAND-GEN-DISPLAY-GOOGLE-ONLINE-PAID-24-25-EN_dis_prs-1_DB-V1_970x250</t>
   </si>
   <si>
     <t>970</t>
   </si>
   <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v1/970x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v1-db&amp;utm_content=970x250&amp;tc_alt=140148" width="970" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140148&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V1-DB_160x600</t>
+    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/09/degree_online/970x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-mim/?utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=701Qu00000D9OyE&amp;utm_term=prs-db-version1&amp;utm_content=970x250&amp;tc_alt=143239" width="970" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=143239&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>iese-eu_v1mp_DEG-MIM-DEMAND-GEN-DISPLAY-GOOGLE-ONLINE-PAID-24-25-EN_dis_prs-1_DB-V1_160x600</t>
   </si>
   <si>
     <t>160</t>
   </si>
   <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v1/160x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v1-db&amp;utm_content=160x600&amp;tc_alt=140149" width="160" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140149&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V1-DB_728x90</t>
+    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/09/degree_online/160x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-mim/?utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=701Qu00000D9OyE&amp;utm_term=prs-db-version1&amp;utm_content=160x600&amp;tc_alt=143240" width="160" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=143240&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>iese-eu_v1mp_DEG-MIM-DEMAND-GEN-DISPLAY-GOOGLE-ONLINE-PAID-24-25-EN_dis_prs-1_DB-V1_728x90</t>
   </si>
   <si>
     <t>728</t>
@@ -1193,694 +1193,115 @@
     <t>90</t>
   </si>
   <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v1/728x90/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v1-db&amp;utm_content=728x90&amp;tc_alt=140150" width="728" height="90" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140150&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V1-RI_300x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v1/300x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v1-ri&amp;utm_content=300x600&amp;tc_alt=140151" width="300" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140151&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V1-RI_300x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v1/300x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v1-ri&amp;utm_content=300x250&amp;tc_alt=140152" width="300" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140152&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V1-RI_320x100</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v1/320x100/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v1-ri&amp;utm_content=320x100&amp;tc_alt=140153" width="320" height="100" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140153&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V1-RI_970x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v1/970x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v1-ri&amp;utm_content=970x250&amp;tc_alt=140154" width="970" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140154&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V1-RI_160x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v1/160x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v1-ri&amp;utm_content=160x600&amp;tc_alt=140155" width="160" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140155&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V1-RI_728x90</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v1/728x90/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v1-ri&amp;utm_content=728x90&amp;tc_alt=140156" width="728" height="90" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140156&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V2-DB_300x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v2/300x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v2-db&amp;utm_content=300x600&amp;tc_alt=140157" width="300" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140157&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V2-DB_300x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v2/300x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v2-db&amp;utm_content=300x250&amp;tc_alt=140158" width="300" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140158&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V2-DB_320x100</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v2/320x100/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v2-db&amp;utm_content=320x100&amp;tc_alt=140159" width="320" height="100" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140159&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V2-DB_970x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v2/970x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v2-db&amp;utm_content=970x250&amp;tc_alt=140160" width="970" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140160&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V2-DB_160x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v2/160x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v2-db&amp;utm_content=160x600&amp;tc_alt=140161" width="160" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140161&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V2-DB_728x90</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v2/728x90/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v2-db&amp;utm_content=728x90&amp;tc_alt=140162" width="728" height="90" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140162&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V2-RI_300x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v2/300x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v2-ri&amp;utm_content=300x600&amp;tc_alt=140163" width="300" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140163&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V2-RI_300x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v2/300x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v2-ri&amp;utm_content=300x250&amp;tc_alt=140164" width="300" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140164&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V2-RI_320x100</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v2/320x100/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v2-ri&amp;utm_content=320x100&amp;tc_alt=140165" width="320" height="100" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140165&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V2-RI_970x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v2/970x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v2-ri&amp;utm_content=970x250&amp;tc_alt=140166" width="970" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140166&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V2-RI_160x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v2/160x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v2-ri&amp;utm_content=160x600&amp;tc_alt=140167" width="160" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140167&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V2-RI_728x90</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v2/728x90/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v2-ri&amp;utm_content=728x90&amp;tc_alt=140168" width="728" height="90" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140168&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V3-DB_300x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v3/300x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v3-db&amp;utm_content=300x600&amp;tc_alt=140169" width="300" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140169&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V3-DB_300x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v3/300x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v3-db&amp;utm_content=300x250&amp;tc_alt=140170" width="300" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140170&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V3-DB_320x100</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v3/320x100/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v3-db&amp;utm_content=320x100&amp;tc_alt=140171" width="320" height="100" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140171&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V3-DB_970x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v3/970x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v3-db&amp;utm_content=970x250&amp;tc_alt=140172" width="970" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140172&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V3-DB_160x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v3/160x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v3-db&amp;utm_content=160x600&amp;tc_alt=140173" width="160" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140173&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V3-DB_728x90</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v3/728x90/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v3-db&amp;utm_content=728x90&amp;tc_alt=140174" width="728" height="90" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140174&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V3-RI_300x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v3/300x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v3-ri&amp;utm_content=300x600&amp;tc_alt=140175" width="300" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140175&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V3-RI_300x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v3/300x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v3-ri&amp;utm_content=300x250&amp;tc_alt=140176" width="300" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140176&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V3-RI_320x100</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v3/320x100/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v3-ri&amp;utm_content=320x100&amp;tc_alt=140177" width="320" height="100" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140177&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V3-RI_970x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v3/970x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v3-ri&amp;utm_content=970x250&amp;tc_alt=140178" width="970" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140178&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V3-RI_160x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v3/160x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v3-ri&amp;utm_content=160x600&amp;tc_alt=140179" width="160" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140179&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V3-RI_728x90</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v3/728x90/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v3-ri&amp;utm_content=728x90&amp;tc_alt=140180" width="728" height="90" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140180&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V4-DB_300x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v4/300x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v4-db&amp;utm_content=300x600&amp;tc_alt=140181" width="300" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140181&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V4-DB_300x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v4/300x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v4-db&amp;utm_content=300x250&amp;tc_alt=140182" width="300" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140182&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V4-DB_320x100</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v4/320x100/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v4-db&amp;utm_content=320x100&amp;tc_alt=140183" width="320" height="100" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140183&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V4-DB_970x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v4/970x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v4-db&amp;utm_content=970x250&amp;tc_alt=140184" width="970" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140184&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V4-DB_160x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v4/160x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v4-db&amp;utm_content=160x600&amp;tc_alt=140185" width="160" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140185&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V4-DB_728x90</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v4/728x90/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v4-db&amp;utm_content=728x90&amp;tc_alt=140186" width="728" height="90" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140186&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V4-RI_300x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v4/300x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v4-ri&amp;utm_content=300x600&amp;tc_alt=140187" width="300" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140187&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V4-RI_300x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v4/300x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v4-ri&amp;utm_content=300x250&amp;tc_alt=140188" width="300" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140188&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V4-RI_320x100</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v4/320x100/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v4-ri&amp;utm_content=320x100&amp;tc_alt=140189" width="320" height="100" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140189&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V4-RI_970x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v4/970x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v4-ri&amp;utm_content=970x250&amp;tc_alt=140190" width="970" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140190&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V4-RI_160x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v4/160x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v4-ri&amp;utm_content=160x600&amp;tc_alt=140191" width="160" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140191&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V4-RI_728x90</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v4/728x90/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v4-ri&amp;utm_content=728x90&amp;tc_alt=140192" width="728" height="90" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140192&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V5-DB_300x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v5/300x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v5-db&amp;utm_content=300x600&amp;tc_alt=140193" width="300" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140193&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V5-DB_300x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v5/300x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v5-db&amp;utm_content=300x250&amp;tc_alt=140194" width="300" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140194&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V5-DB_320x100</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v5/320x100/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v5-db&amp;utm_content=320x100&amp;tc_alt=140195" width="320" height="100" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140195&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V5-DB_970x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v5/970x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v5-db&amp;utm_content=970x250&amp;tc_alt=140196" width="970" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140196&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V5-DB_160x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v5/160x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v5-db&amp;utm_content=160x600&amp;tc_alt=140197" width="160" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140197&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V5-DB_728x90</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v5/728x90/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v5-db&amp;utm_content=728x90&amp;tc_alt=140198" width="728" height="90" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140198&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V5-RI_300x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v5/300x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v5-ri&amp;utm_content=300x600&amp;tc_alt=140199" width="300" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140199&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V5-RI_300x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v5/300x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v5-ri&amp;utm_content=300x250&amp;tc_alt=140200" width="300" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140200&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V5-RI_320x100</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v5/320x100/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v5-ri&amp;utm_content=320x100&amp;tc_alt=140201" width="320" height="100" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140201&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V5-RI_970x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v5/970x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v5-ri&amp;utm_content=970x250&amp;tc_alt=140202" width="970" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140202&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V5-RI_160x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v5/160x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v5-ri&amp;utm_content=160x600&amp;tc_alt=140203" width="160" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140203&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_prs-1_V5-RI_728x90</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v5/728x90/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DN7PW&amp;utm_term=v5-ri&amp;utm_content=728x90&amp;tc_alt=140204" width="728" height="90" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140204&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V1-DB_300x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v1/300x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v1-db&amp;utm_content=300x600&amp;tc_alt=140205" width="300" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140205&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V1-DB_300x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v1/300x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v1-db&amp;utm_content=300x250&amp;tc_alt=140206" width="300" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140206&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V1-DB_320x100</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v1/320x100/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v1-db&amp;utm_content=320x100&amp;tc_alt=140207" width="320" height="100" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140207&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V1-DB_970x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v1/970x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v1-db&amp;utm_content=970x250&amp;tc_alt=140208" width="970" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140208&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V1-DB_160x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v1/160x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v1-db&amp;utm_content=160x600&amp;tc_alt=140209" width="160" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140209&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V1-DB_728x90</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v1/728x90/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v1-db&amp;utm_content=728x90&amp;tc_alt=140210" width="728" height="90" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140210&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V1-RI_300x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v1/300x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v1-ri&amp;utm_content=300x600&amp;tc_alt=140211" width="300" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140211&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V1-RI_300x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v1/300x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v1-ri&amp;utm_content=300x250&amp;tc_alt=140212" width="300" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140212&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V1-RI_320x100</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v1/320x100/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v1-ri&amp;utm_content=320x100&amp;tc_alt=140213" width="320" height="100" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140213&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V1-RI_970x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v1/970x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v1-ri&amp;utm_content=970x250&amp;tc_alt=140214" width="970" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140214&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V1-RI_160x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v1/160x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v1-ri&amp;utm_content=160x600&amp;tc_alt=140215" width="160" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140215&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V1-RI_728x90</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v1/728x90/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v1-ri&amp;utm_content=728x90&amp;tc_alt=140216" width="728" height="90" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140216&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V2-DB_300x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v2/300x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v2-db&amp;utm_content=300x600&amp;tc_alt=140217" width="300" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140217&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V2-DB_300x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v2/300x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v2-db&amp;utm_content=300x250&amp;tc_alt=140218" width="300" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140218&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V2-DB_320x100</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v2/320x100/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v2-db&amp;utm_content=320x100&amp;tc_alt=140219" width="320" height="100" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140219&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V2-DB_970x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v2/970x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v2-db&amp;utm_content=970x250&amp;tc_alt=140220" width="970" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140220&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V2-DB_160x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v2/160x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v2-db&amp;utm_content=160x600&amp;tc_alt=140221" width="160" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140221&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V2-DB_728x90</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v2/728x90/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v2-db&amp;utm_content=728x90&amp;tc_alt=140222" width="728" height="90" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140222&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V2-RI_300x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v2/300x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v2-ri&amp;utm_content=300x600&amp;tc_alt=140223" width="300" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140223&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V2-RI_300x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v2/300x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v2-ri&amp;utm_content=300x250&amp;tc_alt=140224" width="300" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140224&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V2-RI_320x100</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v2/320x100/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v2-ri&amp;utm_content=320x100&amp;tc_alt=140225" width="320" height="100" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140225&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V2-RI_970x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v2/970x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v2-ri&amp;utm_content=970x250&amp;tc_alt=140226" width="970" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140226&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V2-RI_160x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v2/160x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v2-ri&amp;utm_content=160x600&amp;tc_alt=140227" width="160" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140227&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V2-RI_728x90</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v2/728x90/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v2-ri&amp;utm_content=728x90&amp;tc_alt=140228" width="728" height="90" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140228&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V3-DB_300x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v3/300x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v3-db&amp;utm_content=300x600&amp;tc_alt=140229" width="300" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140229&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V3-DB_300x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v3/300x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v3-db&amp;utm_content=300x250&amp;tc_alt=140230" width="300" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140230&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V3-DB_320x100</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v3/320x100/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v3-db&amp;utm_content=320x100&amp;tc_alt=140231" width="320" height="100" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140231&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V3-DB_970x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v3/970x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v3-db&amp;utm_content=970x250&amp;tc_alt=140232" width="970" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140232&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V3-DB_160x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v3/160x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v3-db&amp;utm_content=160x600&amp;tc_alt=140233" width="160" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140233&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V3-DB_728x90</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v3/728x90/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v3-db&amp;utm_content=728x90&amp;tc_alt=140234" width="728" height="90" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140234&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V3-RI_300x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v3/300x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v3-ri&amp;utm_content=300x600&amp;tc_alt=140235" width="300" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140235&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V3-RI_300x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v3/300x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v3-ri&amp;utm_content=300x250&amp;tc_alt=140236" width="300" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140236&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V3-RI_320x100</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v3/320x100/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v3-ri&amp;utm_content=320x100&amp;tc_alt=140237" width="320" height="100" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140237&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V3-RI_970x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v3/970x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v3-ri&amp;utm_content=970x250&amp;tc_alt=140238" width="970" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140238&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V3-RI_160x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v3/160x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v3-ri&amp;utm_content=160x600&amp;tc_alt=140239" width="160" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140239&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V3-RI_728x90</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v3/728x90/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=display&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v3-ri&amp;utm_content=728x90&amp;tc_alt=140240" width="728" height="90" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140240&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V4-DB_300x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v4/300x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=dis-rtg-1&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v4-db&amp;utm_content=300x600&amp;tc_alt=140241" width="300" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140241&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V4-DB_300x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v4/300x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=dis-rtg-1&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v4-db&amp;utm_content=300x250&amp;tc_alt=140242" width="300" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140242&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V4-DB_320x100</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v4/320x100/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=dis-rtg-1&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v4-db&amp;utm_content=320x100&amp;tc_alt=140243" width="320" height="100" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140243&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V4-DB_970x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v4/970x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=dis-rtg-1&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v4-db&amp;utm_content=970x250&amp;tc_alt=140244" width="970" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140244&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V4-DB_160x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v4/160x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=dis-rtg-1&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v4-db&amp;utm_content=160x600&amp;tc_alt=140245" width="160" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140245&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V4-DB_728x90</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v4/728x90/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=dis-rtg-1&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v4-db&amp;utm_content=728x90&amp;tc_alt=140246" width="728" height="90" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140246&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V4-RI_300x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v4/300x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=dis-rtg-1&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v4-ri&amp;utm_content=300x600&amp;tc_alt=140247" width="300" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140247&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V4-RI_300x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v4/300x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=dis-rtg-1&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v4-ri&amp;utm_content=300x250&amp;tc_alt=140248" width="300" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140248&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V4-RI_320x100</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v4/320x100/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=dis-rtg-1&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v4-ri&amp;utm_content=320x100&amp;tc_alt=140249" width="320" height="100" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140249&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V4-RI_970x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v4/970x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=dis-rtg-1&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v4-ri&amp;utm_content=970x250&amp;tc_alt=140250" width="970" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140250&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V4-RI_160x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v4/160x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=dis-rtg-1&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v4-ri&amp;utm_content=160x600&amp;tc_alt=140251" width="160" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140251&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V4-RI_728x90</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v4/728x90/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=dis-rtg-1&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v4-ri&amp;utm_content=728x90&amp;tc_alt=140252" width="728" height="90" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140252&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V5-DB_300x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v5/300x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=dis-rtg-1&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v5-db&amp;utm_content=300x600&amp;tc_alt=140253" width="300" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140253&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V5-DB_300x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v5/300x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=dis-rtg-1&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v5-db&amp;utm_content=300x250&amp;tc_alt=140254" width="300" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140254&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V5-DB_320x100</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v5/320x100/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=dis-rtg-1&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v5-db&amp;utm_content=320x100&amp;tc_alt=140255" width="320" height="100" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140255&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V5-DB_970x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v5/970x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=dis-rtg-1&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v5-db&amp;utm_content=970x250&amp;tc_alt=140256" width="970" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140256&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V5-DB_160x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v5/160x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=dis-rtg-1&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v5-db&amp;utm_content=160x600&amp;tc_alt=140257" width="160" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140257&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V5-DB_728x90</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v5/728x90/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw/?utm_source=google&amp;utm_medium=dis-rtg-1&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v5-db&amp;utm_content=728x90&amp;tc_alt=140258" width="728" height="90" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140258&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V5-RI_300x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v5/300x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=dis-rtg-1&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v5-ri&amp;utm_content=300x600&amp;tc_alt=140259" width="300" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140259&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V5-RI_300x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v5/300x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=dis-rtg-1&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v5-ri&amp;utm_content=300x250&amp;tc_alt=140260" width="300" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140260&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V5-RI_320x100</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v5/320x100/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=dis-rtg-1&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v5-ri&amp;utm_content=320x100&amp;tc_alt=140261" width="320" height="100" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140261&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V5-RI_970x250</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v5/970x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=dis-rtg-1&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v5-ri&amp;utm_content=970x250&amp;tc_alt=140262" width="970" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140262&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V5-RI_160x600</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v5/160x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=dis-rtg-1&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v5-ri&amp;utm_content=160x600&amp;tc_alt=140263" width="160" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140263&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>iese-pl_v1mp_IEP-LAE-DACH-CONSIDERATION_dis_rtg-1_V5-RI_728x90</t>
-  </si>
-  <si>
-    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/07/consideration/v5/728x90/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-artificial-intelligence-warsaw-interview/?utm_source=google&amp;utm_medium=dis-rtg-1&amp;utm_campaign=701Qu00000DMvOZ&amp;utm_term=v5-ri&amp;utm_content=728x90&amp;tc_alt=140264" width="728" height="90" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=140264&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
+    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/09/degree_online/728x90/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-mim/?utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=701Qu00000D9OyE&amp;utm_term=prs-db-version1&amp;utm_content=728x90&amp;tc_alt=143241" width="728" height="90" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=143241&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>iese-eu_v1mp_DEG-MIM-DEMAND-GEN-DISPLAY-GOOGLE-ONLINE-PAID-24-25-EN_dis_rtg-1_DB-V1_300x600</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/09/degree_online/300x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-mim/?utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=701Qu00000D9OyE&amp;utm_term=rtg-db-version1&amp;utm_content=300x600&amp;tc_alt=143242" width="300" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=143242&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>iese-eu_v1mp_DEG-MIM-DEMAND-GEN-DISPLAY-GOOGLE-ONLINE-PAID-24-25-EN_dis_rtg-1_DB-V1_300x250</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/09/degree_online/300x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-mim/?utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=701Qu00000D9OyE&amp;utm_term=rtg-db-version1&amp;utm_content=300x250&amp;tc_alt=143243" width="300" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=143243&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>iese-eu_v1mp_DEG-MIM-DEMAND-GEN-DISPLAY-GOOGLE-ONLINE-PAID-24-25-EN_dis_rtg-1_DB-V1_320x100</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/09/degree_online/320x100/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-mim/?utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=701Qu00000D9OyE&amp;utm_term=rtg-db-version1&amp;utm_content=320x100&amp;tc_alt=143244" width="320" height="100" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=143244&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>iese-eu_v1mp_DEG-MIM-DEMAND-GEN-DISPLAY-GOOGLE-ONLINE-PAID-24-25-EN_dis_rtg-1_DB-V1_970x250</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/09/degree_online/970x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-mim/?utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=701Qu00000D9OyE&amp;utm_term=rtg-db-version1&amp;utm_content=970x250&amp;tc_alt=143245" width="970" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=143245&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>iese-eu_v1mp_DEG-MIM-DEMAND-GEN-DISPLAY-GOOGLE-ONLINE-PAID-24-25-EN_dis_rtg-1_DB-V1_160x600</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/09/degree_online/160x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-mim/?utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=701Qu00000D9OyE&amp;utm_term=rtg-db-version1&amp;utm_content=160x600&amp;tc_alt=143246" width="160" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=143246&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>iese-eu_v1mp_DEG-MIM-DEMAND-GEN-DISPLAY-GOOGLE-ONLINE-PAID-24-25-EN_dis_rtg-1_DB-V1_728x90</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/09/degree_online/728x90/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-mim/?utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=701Qu00000D9OyE&amp;utm_term=rtg-db-version1&amp;utm_content=728x90&amp;tc_alt=143247" width="728" height="90" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=143247&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>iese-eu_v1mp_DEG-MIM-DEMAND-GEN-DISPLAY-GOOGLE-ONLINE-PAID-24-25-EN_dis_prs-1_DB-V2_300x600</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/09/degree_online/300x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-mim/?utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=701Qu00000D9OyE&amp;utm_term=prs-db-version2&amp;utm_content=300x600&amp;tc_alt=143248" width="300" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=143248&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>iese-eu_v1mp_DEG-MIM-DEMAND-GEN-DISPLAY-GOOGLE-ONLINE-PAID-24-25-EN_dis_prs-1_DB-V2_300x250</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/09/degree_online/300x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-mim/?utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=701Qu00000D9OyE&amp;utm_term=prs-db-version2&amp;utm_content=300x250&amp;tc_alt=143249" width="300" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=143249&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>iese-eu_v1mp_DEG-MIM-DEMAND-GEN-DISPLAY-GOOGLE-ONLINE-PAID-24-25-EN_dis_prs-1_DB-V2_320x100</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/09/degree_online/320x100/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-mim/?utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=701Qu00000D9OyE&amp;utm_term=prs-db-version2&amp;utm_content=320x100&amp;tc_alt=143250" width="320" height="100" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=143250&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>iese-eu_v1mp_DEG-MIM-DEMAND-GEN-DISPLAY-GOOGLE-ONLINE-PAID-24-25-EN_dis_prs-1_DB-V2_970x250</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/09/degree_online/970x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-mim/?utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=701Qu00000D9OyE&amp;utm_term=prs-db-version2&amp;utm_content=970x250&amp;tc_alt=143251" width="970" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=143251&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>iese-eu_v1mp_DEG-MIM-DEMAND-GEN-DISPLAY-GOOGLE-ONLINE-PAID-24-25-EN_dis_prs-1_DB-V2_160x600</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/09/degree_online/160x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-mim/?utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=701Qu00000D9OyE&amp;utm_term=prs-db-version2&amp;utm_content=160x600&amp;tc_alt=143252" width="160" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=143252&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>iese-eu_v1mp_DEG-MIM-DEMAND-GEN-DISPLAY-GOOGLE-ONLINE-PAID-24-25-EN_dis_prs-1_DB-V2_728x90</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/09/degree_online/728x90/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-mim/?utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=701Qu00000D9OyE&amp;utm_term=prs-db-version2&amp;utm_content=728x90&amp;tc_alt=143253" width="728" height="90" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=143253&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>iese-eu_v1mp_DEG-MIM-DEMAND-GEN-DISPLAY-GOOGLE-ONLINE-PAID-24-25-EN_dis_rtg-1_DB-V2_300x600</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/09/degree_online/300x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-mim/?utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=701Qu00000D9OyE&amp;utm_term=rtg-db-version2&amp;utm_content=300x600&amp;tc_alt=143254" width="300" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=143254&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>iese-eu_v1mp_DEG-MIM-DEMAND-GEN-DISPLAY-GOOGLE-ONLINE-PAID-24-25-EN_dis_rtg-1_DB-V2_300x250</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/09/degree_online/300x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-mim/?utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=701Qu00000D9OyE&amp;utm_term=rtg-db-version2&amp;utm_content=300x250&amp;tc_alt=143255" width="300" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=143255&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>iese-eu_v1mp_DEG-MIM-DEMAND-GEN-DISPLAY-GOOGLE-ONLINE-PAID-24-25-EN_dis_rtg-1_DB-V2_320x100</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/09/degree_online/320x100/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-mim/?utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=701Qu00000D9OyE&amp;utm_term=rtg-db-version2&amp;utm_content=320x100&amp;tc_alt=143256" width="320" height="100" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=143256&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>iese-eu_v1mp_DEG-MIM-DEMAND-GEN-DISPLAY-GOOGLE-ONLINE-PAID-24-25-EN_dis_rtg-1_DB-V2_970x250</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/09/degree_online/970x250/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-mim/?utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=701Qu00000D9OyE&amp;utm_term=rtg-db-version2&amp;utm_content=970x250&amp;tc_alt=143257" width="970" height="250" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=143257&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>iese-eu_v1mp_DEG-MIM-DEMAND-GEN-DISPLAY-GOOGLE-ONLINE-PAID-24-25-EN_dis_rtg-1_DB-V2_160x600</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/09/degree_online/160x600/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-mim/?utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=701Qu00000D9OyE&amp;utm_term=rtg-db-version2&amp;utm_content=160x600&amp;tc_alt=143258" width="160" height="600" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=143258&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>iese-eu_v1mp_DEG-MIM-DEMAND-GEN-DISPLAY-GOOGLE-ONLINE-PAID-24-25-EN_dis_rtg-1_DB-V2_728x90</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://ppj05.cdnwebcloud.com/IESE/2024/09/degree_online/728x90/index.html?n_o_ct=%%TTD_CLK_ESC%%&amp;link=https://formscloud.iese.edu/landings-mim/?utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=701Qu00000D9OyE&amp;utm_term=rtg-db-version2&amp;utm_content=728x90&amp;tc_alt=143259" width="728" height="90" frameborder="0" scrolling="no" marginheight="0" marginwidth="0"&gt;&lt;/iframe&gt;&lt;script type="text/javascript" src="//bucket.cdnwebcloud.com/n_one_vway_IESE%20Business%20School.js?tc=143259&amp;n_o_ord=%%TTD_CACHEBUSTER%%"&gt;&lt;/script&gt;</t>
   </si>
 </sst>
 </file>
@@ -4284,7 +3705,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X121"/>
+  <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4498,7 +3919,7 @@
         <v>389</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>390</v>
+        <v>369</v>
       </c>
       <c r="J8" t="s">
         <v>370</v>
@@ -4506,7 +3927,7 @@
     </row>
     <row r="9" spans="1:24">
       <c r="A9" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C9" t="s">
         <v>366</v>
@@ -4515,10 +3936,10 @@
         <v>372</v>
       </c>
       <c r="E9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>390</v>
+        <v>369</v>
       </c>
       <c r="J9" t="s">
         <v>370</v>
@@ -4526,7 +3947,7 @@
     </row>
     <row r="10" spans="1:24">
       <c r="A10" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C10" t="s">
         <v>375</v>
@@ -4535,10 +3956,10 @@
         <v>376</v>
       </c>
       <c r="E10" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>390</v>
+        <v>369</v>
       </c>
       <c r="J10" t="s">
         <v>370</v>
@@ -4546,7 +3967,7 @@
     </row>
     <row r="11" spans="1:24">
       <c r="A11" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C11" t="s">
         <v>379</v>
@@ -4555,10 +3976,10 @@
         <v>372</v>
       </c>
       <c r="E11" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>390</v>
+        <v>369</v>
       </c>
       <c r="J11" t="s">
         <v>370</v>
@@ -4566,7 +3987,7 @@
     </row>
     <row r="12" spans="1:24">
       <c r="A12" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C12" t="s">
         <v>382</v>
@@ -4575,10 +3996,10 @@
         <v>367</v>
       </c>
       <c r="E12" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>390</v>
+        <v>369</v>
       </c>
       <c r="J12" t="s">
         <v>370</v>
@@ -4586,7 +4007,7 @@
     </row>
     <row r="13" spans="1:24">
       <c r="A13" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C13" t="s">
         <v>385</v>
@@ -4595,10 +4016,10 @@
         <v>386</v>
       </c>
       <c r="E13" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>390</v>
+        <v>369</v>
       </c>
       <c r="J13" t="s">
         <v>370</v>
@@ -4606,7 +4027,7 @@
     </row>
     <row r="14" spans="1:24">
       <c r="A14" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C14" t="s">
         <v>366</v>
@@ -4615,7 +4036,7 @@
         <v>367</v>
       </c>
       <c r="E14" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>369</v>
@@ -4626,7 +4047,7 @@
     </row>
     <row r="15" spans="1:24">
       <c r="A15" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C15" t="s">
         <v>366</v>
@@ -4635,7 +4056,7 @@
         <v>372</v>
       </c>
       <c r="E15" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>369</v>
@@ -4646,7 +4067,7 @@
     </row>
     <row r="16" spans="1:24">
       <c r="A16" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C16" t="s">
         <v>375</v>
@@ -4655,7 +4076,7 @@
         <v>376</v>
       </c>
       <c r="E16" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>369</v>
@@ -4666,7 +4087,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C17" t="s">
         <v>379</v>
@@ -4675,7 +4096,7 @@
         <v>372</v>
       </c>
       <c r="E17" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>369</v>
@@ -4686,7 +4107,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C18" t="s">
         <v>382</v>
@@ -4695,7 +4116,7 @@
         <v>367</v>
       </c>
       <c r="E18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>369</v>
@@ -4706,7 +4127,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C19" t="s">
         <v>385</v>
@@ -4715,7 +4136,7 @@
         <v>386</v>
       </c>
       <c r="E19" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>369</v>
@@ -4726,7 +4147,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C20" t="s">
         <v>366</v>
@@ -4735,10 +4156,10 @@
         <v>367</v>
       </c>
       <c r="E20" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>390</v>
+        <v>369</v>
       </c>
       <c r="J20" t="s">
         <v>370</v>
@@ -4746,7 +4167,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C21" t="s">
         <v>366</v>
@@ -4755,10 +4176,10 @@
         <v>372</v>
       </c>
       <c r="E21" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>390</v>
+        <v>369</v>
       </c>
       <c r="J21" t="s">
         <v>370</v>
@@ -4766,7 +4187,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C22" t="s">
         <v>375</v>
@@ -4775,10 +4196,10 @@
         <v>376</v>
       </c>
       <c r="E22" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>390</v>
+        <v>369</v>
       </c>
       <c r="J22" t="s">
         <v>370</v>
@@ -4786,7 +4207,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C23" t="s">
         <v>379</v>
@@ -4795,10 +4216,10 @@
         <v>372</v>
       </c>
       <c r="E23" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>390</v>
+        <v>369</v>
       </c>
       <c r="J23" t="s">
         <v>370</v>
@@ -4806,7 +4227,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C24" t="s">
         <v>382</v>
@@ -4815,10 +4236,10 @@
         <v>367</v>
       </c>
       <c r="E24" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>390</v>
+        <v>369</v>
       </c>
       <c r="J24" t="s">
         <v>370</v>
@@ -4826,7 +4247,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C25" t="s">
         <v>385</v>
@@ -4835,1932 +4256,12 @@
         <v>386</v>
       </c>
       <c r="E25" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>390</v>
+        <v>369</v>
       </c>
       <c r="J25" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" t="s">
-        <v>425</v>
-      </c>
-      <c r="C26" t="s">
-        <v>366</v>
-      </c>
-      <c r="D26" t="s">
-        <v>367</v>
-      </c>
-      <c r="E26" t="s">
-        <v>426</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J26" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" t="s">
-        <v>427</v>
-      </c>
-      <c r="C27" t="s">
-        <v>366</v>
-      </c>
-      <c r="D27" t="s">
-        <v>372</v>
-      </c>
-      <c r="E27" t="s">
-        <v>428</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J27" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="A28" t="s">
-        <v>429</v>
-      </c>
-      <c r="C28" t="s">
-        <v>375</v>
-      </c>
-      <c r="D28" t="s">
-        <v>376</v>
-      </c>
-      <c r="E28" t="s">
-        <v>430</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J28" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" t="s">
-        <v>431</v>
-      </c>
-      <c r="C29" t="s">
-        <v>379</v>
-      </c>
-      <c r="D29" t="s">
-        <v>372</v>
-      </c>
-      <c r="E29" t="s">
-        <v>432</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J29" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30" t="s">
-        <v>433</v>
-      </c>
-      <c r="C30" t="s">
-        <v>382</v>
-      </c>
-      <c r="D30" t="s">
-        <v>367</v>
-      </c>
-      <c r="E30" t="s">
-        <v>434</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J30" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="A31" t="s">
-        <v>435</v>
-      </c>
-      <c r="C31" t="s">
-        <v>385</v>
-      </c>
-      <c r="D31" t="s">
-        <v>386</v>
-      </c>
-      <c r="E31" t="s">
-        <v>436</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J31" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32" t="s">
-        <v>437</v>
-      </c>
-      <c r="C32" t="s">
-        <v>366</v>
-      </c>
-      <c r="D32" t="s">
-        <v>367</v>
-      </c>
-      <c r="E32" t="s">
-        <v>438</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J32" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="A33" t="s">
-        <v>439</v>
-      </c>
-      <c r="C33" t="s">
-        <v>366</v>
-      </c>
-      <c r="D33" t="s">
-        <v>372</v>
-      </c>
-      <c r="E33" t="s">
-        <v>440</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J33" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10">
-      <c r="A34" t="s">
-        <v>441</v>
-      </c>
-      <c r="C34" t="s">
-        <v>375</v>
-      </c>
-      <c r="D34" t="s">
-        <v>376</v>
-      </c>
-      <c r="E34" t="s">
-        <v>442</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J34" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10">
-      <c r="A35" t="s">
-        <v>443</v>
-      </c>
-      <c r="C35" t="s">
-        <v>379</v>
-      </c>
-      <c r="D35" t="s">
-        <v>372</v>
-      </c>
-      <c r="E35" t="s">
-        <v>444</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J35" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10">
-      <c r="A36" t="s">
-        <v>445</v>
-      </c>
-      <c r="C36" t="s">
-        <v>382</v>
-      </c>
-      <c r="D36" t="s">
-        <v>367</v>
-      </c>
-      <c r="E36" t="s">
-        <v>446</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J36" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10">
-      <c r="A37" t="s">
-        <v>447</v>
-      </c>
-      <c r="C37" t="s">
-        <v>385</v>
-      </c>
-      <c r="D37" t="s">
-        <v>386</v>
-      </c>
-      <c r="E37" t="s">
-        <v>448</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J37" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10">
-      <c r="A38" t="s">
-        <v>449</v>
-      </c>
-      <c r="C38" t="s">
-        <v>366</v>
-      </c>
-      <c r="D38" t="s">
-        <v>367</v>
-      </c>
-      <c r="E38" t="s">
-        <v>450</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J38" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10">
-      <c r="A39" t="s">
-        <v>451</v>
-      </c>
-      <c r="C39" t="s">
-        <v>366</v>
-      </c>
-      <c r="D39" t="s">
-        <v>372</v>
-      </c>
-      <c r="E39" t="s">
-        <v>452</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J39" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10">
-      <c r="A40" t="s">
-        <v>453</v>
-      </c>
-      <c r="C40" t="s">
-        <v>375</v>
-      </c>
-      <c r="D40" t="s">
-        <v>376</v>
-      </c>
-      <c r="E40" t="s">
-        <v>454</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J40" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10">
-      <c r="A41" t="s">
-        <v>455</v>
-      </c>
-      <c r="C41" t="s">
-        <v>379</v>
-      </c>
-      <c r="D41" t="s">
-        <v>372</v>
-      </c>
-      <c r="E41" t="s">
-        <v>456</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J41" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10">
-      <c r="A42" t="s">
-        <v>457</v>
-      </c>
-      <c r="C42" t="s">
-        <v>382</v>
-      </c>
-      <c r="D42" t="s">
-        <v>367</v>
-      </c>
-      <c r="E42" t="s">
-        <v>458</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J42" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10">
-      <c r="A43" t="s">
-        <v>459</v>
-      </c>
-      <c r="C43" t="s">
-        <v>385</v>
-      </c>
-      <c r="D43" t="s">
-        <v>386</v>
-      </c>
-      <c r="E43" t="s">
-        <v>460</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J43" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10">
-      <c r="A44" t="s">
-        <v>461</v>
-      </c>
-      <c r="C44" t="s">
-        <v>366</v>
-      </c>
-      <c r="D44" t="s">
-        <v>367</v>
-      </c>
-      <c r="E44" t="s">
-        <v>462</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J44" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10">
-      <c r="A45" t="s">
-        <v>463</v>
-      </c>
-      <c r="C45" t="s">
-        <v>366</v>
-      </c>
-      <c r="D45" t="s">
-        <v>372</v>
-      </c>
-      <c r="E45" t="s">
-        <v>464</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J45" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10">
-      <c r="A46" t="s">
-        <v>465</v>
-      </c>
-      <c r="C46" t="s">
-        <v>375</v>
-      </c>
-      <c r="D46" t="s">
-        <v>376</v>
-      </c>
-      <c r="E46" t="s">
-        <v>466</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J46" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10">
-      <c r="A47" t="s">
-        <v>467</v>
-      </c>
-      <c r="C47" t="s">
-        <v>379</v>
-      </c>
-      <c r="D47" t="s">
-        <v>372</v>
-      </c>
-      <c r="E47" t="s">
-        <v>468</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J47" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10">
-      <c r="A48" t="s">
-        <v>469</v>
-      </c>
-      <c r="C48" t="s">
-        <v>382</v>
-      </c>
-      <c r="D48" t="s">
-        <v>367</v>
-      </c>
-      <c r="E48" t="s">
-        <v>470</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J48" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10">
-      <c r="A49" t="s">
-        <v>471</v>
-      </c>
-      <c r="C49" t="s">
-        <v>385</v>
-      </c>
-      <c r="D49" t="s">
-        <v>386</v>
-      </c>
-      <c r="E49" t="s">
-        <v>472</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J49" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10">
-      <c r="A50" t="s">
-        <v>473</v>
-      </c>
-      <c r="C50" t="s">
-        <v>366</v>
-      </c>
-      <c r="D50" t="s">
-        <v>367</v>
-      </c>
-      <c r="E50" t="s">
-        <v>474</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J50" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10">
-      <c r="A51" t="s">
-        <v>475</v>
-      </c>
-      <c r="C51" t="s">
-        <v>366</v>
-      </c>
-      <c r="D51" t="s">
-        <v>372</v>
-      </c>
-      <c r="E51" t="s">
-        <v>476</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J51" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10">
-      <c r="A52" t="s">
-        <v>477</v>
-      </c>
-      <c r="C52" t="s">
-        <v>375</v>
-      </c>
-      <c r="D52" t="s">
-        <v>376</v>
-      </c>
-      <c r="E52" t="s">
-        <v>478</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J52" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10">
-      <c r="A53" t="s">
-        <v>479</v>
-      </c>
-      <c r="C53" t="s">
-        <v>379</v>
-      </c>
-      <c r="D53" t="s">
-        <v>372</v>
-      </c>
-      <c r="E53" t="s">
-        <v>480</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J53" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10">
-      <c r="A54" t="s">
-        <v>481</v>
-      </c>
-      <c r="C54" t="s">
-        <v>382</v>
-      </c>
-      <c r="D54" t="s">
-        <v>367</v>
-      </c>
-      <c r="E54" t="s">
-        <v>482</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J54" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10">
-      <c r="A55" t="s">
-        <v>483</v>
-      </c>
-      <c r="C55" t="s">
-        <v>385</v>
-      </c>
-      <c r="D55" t="s">
-        <v>386</v>
-      </c>
-      <c r="E55" t="s">
-        <v>484</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J55" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10">
-      <c r="A56" t="s">
-        <v>485</v>
-      </c>
-      <c r="C56" t="s">
-        <v>366</v>
-      </c>
-      <c r="D56" t="s">
-        <v>367</v>
-      </c>
-      <c r="E56" t="s">
-        <v>486</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J56" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10">
-      <c r="A57" t="s">
-        <v>487</v>
-      </c>
-      <c r="C57" t="s">
-        <v>366</v>
-      </c>
-      <c r="D57" t="s">
-        <v>372</v>
-      </c>
-      <c r="E57" t="s">
-        <v>488</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J57" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10">
-      <c r="A58" t="s">
-        <v>489</v>
-      </c>
-      <c r="C58" t="s">
-        <v>375</v>
-      </c>
-      <c r="D58" t="s">
-        <v>376</v>
-      </c>
-      <c r="E58" t="s">
-        <v>490</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J58" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10">
-      <c r="A59" t="s">
-        <v>491</v>
-      </c>
-      <c r="C59" t="s">
-        <v>379</v>
-      </c>
-      <c r="D59" t="s">
-        <v>372</v>
-      </c>
-      <c r="E59" t="s">
-        <v>492</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J59" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10">
-      <c r="A60" t="s">
-        <v>493</v>
-      </c>
-      <c r="C60" t="s">
-        <v>382</v>
-      </c>
-      <c r="D60" t="s">
-        <v>367</v>
-      </c>
-      <c r="E60" t="s">
-        <v>494</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J60" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10">
-      <c r="A61" t="s">
-        <v>495</v>
-      </c>
-      <c r="C61" t="s">
-        <v>385</v>
-      </c>
-      <c r="D61" t="s">
-        <v>386</v>
-      </c>
-      <c r="E61" t="s">
-        <v>496</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J61" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10">
-      <c r="A62" t="s">
-        <v>497</v>
-      </c>
-      <c r="C62" t="s">
-        <v>366</v>
-      </c>
-      <c r="D62" t="s">
-        <v>367</v>
-      </c>
-      <c r="E62" t="s">
-        <v>498</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J62" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10">
-      <c r="A63" t="s">
-        <v>499</v>
-      </c>
-      <c r="C63" t="s">
-        <v>366</v>
-      </c>
-      <c r="D63" t="s">
-        <v>372</v>
-      </c>
-      <c r="E63" t="s">
-        <v>500</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J63" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10">
-      <c r="A64" t="s">
-        <v>501</v>
-      </c>
-      <c r="C64" t="s">
-        <v>375</v>
-      </c>
-      <c r="D64" t="s">
-        <v>376</v>
-      </c>
-      <c r="E64" t="s">
-        <v>502</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J64" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10">
-      <c r="A65" t="s">
-        <v>503</v>
-      </c>
-      <c r="C65" t="s">
-        <v>379</v>
-      </c>
-      <c r="D65" t="s">
-        <v>372</v>
-      </c>
-      <c r="E65" t="s">
-        <v>504</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J65" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10">
-      <c r="A66" t="s">
-        <v>505</v>
-      </c>
-      <c r="C66" t="s">
-        <v>382</v>
-      </c>
-      <c r="D66" t="s">
-        <v>367</v>
-      </c>
-      <c r="E66" t="s">
-        <v>506</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J66" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10">
-      <c r="A67" t="s">
-        <v>507</v>
-      </c>
-      <c r="C67" t="s">
-        <v>385</v>
-      </c>
-      <c r="D67" t="s">
-        <v>386</v>
-      </c>
-      <c r="E67" t="s">
-        <v>508</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J67" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10">
-      <c r="A68" t="s">
-        <v>509</v>
-      </c>
-      <c r="C68" t="s">
-        <v>366</v>
-      </c>
-      <c r="D68" t="s">
-        <v>367</v>
-      </c>
-      <c r="E68" t="s">
-        <v>510</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J68" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10">
-      <c r="A69" t="s">
-        <v>511</v>
-      </c>
-      <c r="C69" t="s">
-        <v>366</v>
-      </c>
-      <c r="D69" t="s">
-        <v>372</v>
-      </c>
-      <c r="E69" t="s">
-        <v>512</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J69" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10">
-      <c r="A70" t="s">
-        <v>513</v>
-      </c>
-      <c r="C70" t="s">
-        <v>375</v>
-      </c>
-      <c r="D70" t="s">
-        <v>376</v>
-      </c>
-      <c r="E70" t="s">
-        <v>514</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J70" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10">
-      <c r="A71" t="s">
-        <v>515</v>
-      </c>
-      <c r="C71" t="s">
-        <v>379</v>
-      </c>
-      <c r="D71" t="s">
-        <v>372</v>
-      </c>
-      <c r="E71" t="s">
-        <v>516</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J71" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10">
-      <c r="A72" t="s">
-        <v>517</v>
-      </c>
-      <c r="C72" t="s">
-        <v>382</v>
-      </c>
-      <c r="D72" t="s">
-        <v>367</v>
-      </c>
-      <c r="E72" t="s">
-        <v>518</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J72" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10">
-      <c r="A73" t="s">
-        <v>519</v>
-      </c>
-      <c r="C73" t="s">
-        <v>385</v>
-      </c>
-      <c r="D73" t="s">
-        <v>386</v>
-      </c>
-      <c r="E73" t="s">
-        <v>520</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J73" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10">
-      <c r="A74" t="s">
-        <v>521</v>
-      </c>
-      <c r="C74" t="s">
-        <v>366</v>
-      </c>
-      <c r="D74" t="s">
-        <v>367</v>
-      </c>
-      <c r="E74" t="s">
-        <v>522</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J74" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10">
-      <c r="A75" t="s">
-        <v>523</v>
-      </c>
-      <c r="C75" t="s">
-        <v>366</v>
-      </c>
-      <c r="D75" t="s">
-        <v>372</v>
-      </c>
-      <c r="E75" t="s">
-        <v>524</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J75" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10">
-      <c r="A76" t="s">
-        <v>525</v>
-      </c>
-      <c r="C76" t="s">
-        <v>375</v>
-      </c>
-      <c r="D76" t="s">
-        <v>376</v>
-      </c>
-      <c r="E76" t="s">
-        <v>526</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J76" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10">
-      <c r="A77" t="s">
-        <v>527</v>
-      </c>
-      <c r="C77" t="s">
-        <v>379</v>
-      </c>
-      <c r="D77" t="s">
-        <v>372</v>
-      </c>
-      <c r="E77" t="s">
-        <v>528</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J77" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10">
-      <c r="A78" t="s">
-        <v>529</v>
-      </c>
-      <c r="C78" t="s">
-        <v>382</v>
-      </c>
-      <c r="D78" t="s">
-        <v>367</v>
-      </c>
-      <c r="E78" t="s">
-        <v>530</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J78" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10">
-      <c r="A79" t="s">
-        <v>531</v>
-      </c>
-      <c r="C79" t="s">
-        <v>385</v>
-      </c>
-      <c r="D79" t="s">
-        <v>386</v>
-      </c>
-      <c r="E79" t="s">
-        <v>532</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J79" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10">
-      <c r="A80" t="s">
-        <v>533</v>
-      </c>
-      <c r="C80" t="s">
-        <v>366</v>
-      </c>
-      <c r="D80" t="s">
-        <v>367</v>
-      </c>
-      <c r="E80" t="s">
-        <v>534</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J80" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10">
-      <c r="A81" t="s">
-        <v>535</v>
-      </c>
-      <c r="C81" t="s">
-        <v>366</v>
-      </c>
-      <c r="D81" t="s">
-        <v>372</v>
-      </c>
-      <c r="E81" t="s">
-        <v>536</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J81" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10">
-      <c r="A82" t="s">
-        <v>537</v>
-      </c>
-      <c r="C82" t="s">
-        <v>375</v>
-      </c>
-      <c r="D82" t="s">
-        <v>376</v>
-      </c>
-      <c r="E82" t="s">
-        <v>538</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J82" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10">
-      <c r="A83" t="s">
-        <v>539</v>
-      </c>
-      <c r="C83" t="s">
-        <v>379</v>
-      </c>
-      <c r="D83" t="s">
-        <v>372</v>
-      </c>
-      <c r="E83" t="s">
-        <v>540</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J83" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10">
-      <c r="A84" t="s">
-        <v>541</v>
-      </c>
-      <c r="C84" t="s">
-        <v>382</v>
-      </c>
-      <c r="D84" t="s">
-        <v>367</v>
-      </c>
-      <c r="E84" t="s">
-        <v>542</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J84" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10">
-      <c r="A85" t="s">
-        <v>543</v>
-      </c>
-      <c r="C85" t="s">
-        <v>385</v>
-      </c>
-      <c r="D85" t="s">
-        <v>386</v>
-      </c>
-      <c r="E85" t="s">
-        <v>544</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J85" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10">
-      <c r="A86" t="s">
-        <v>545</v>
-      </c>
-      <c r="C86" t="s">
-        <v>366</v>
-      </c>
-      <c r="D86" t="s">
-        <v>367</v>
-      </c>
-      <c r="E86" t="s">
-        <v>546</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J86" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10">
-      <c r="A87" t="s">
-        <v>547</v>
-      </c>
-      <c r="C87" t="s">
-        <v>366</v>
-      </c>
-      <c r="D87" t="s">
-        <v>372</v>
-      </c>
-      <c r="E87" t="s">
-        <v>548</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J87" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10">
-      <c r="A88" t="s">
-        <v>549</v>
-      </c>
-      <c r="C88" t="s">
-        <v>375</v>
-      </c>
-      <c r="D88" t="s">
-        <v>376</v>
-      </c>
-      <c r="E88" t="s">
-        <v>550</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J88" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10">
-      <c r="A89" t="s">
-        <v>551</v>
-      </c>
-      <c r="C89" t="s">
-        <v>379</v>
-      </c>
-      <c r="D89" t="s">
-        <v>372</v>
-      </c>
-      <c r="E89" t="s">
-        <v>552</v>
-      </c>
-      <c r="F89" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J89" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10">
-      <c r="A90" t="s">
-        <v>553</v>
-      </c>
-      <c r="C90" t="s">
-        <v>382</v>
-      </c>
-      <c r="D90" t="s">
-        <v>367</v>
-      </c>
-      <c r="E90" t="s">
-        <v>554</v>
-      </c>
-      <c r="F90" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J90" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10">
-      <c r="A91" t="s">
-        <v>555</v>
-      </c>
-      <c r="C91" t="s">
-        <v>385</v>
-      </c>
-      <c r="D91" t="s">
-        <v>386</v>
-      </c>
-      <c r="E91" t="s">
-        <v>556</v>
-      </c>
-      <c r="F91" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J91" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10">
-      <c r="A92" t="s">
-        <v>557</v>
-      </c>
-      <c r="C92" t="s">
-        <v>366</v>
-      </c>
-      <c r="D92" t="s">
-        <v>367</v>
-      </c>
-      <c r="E92" t="s">
-        <v>558</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J92" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10">
-      <c r="A93" t="s">
-        <v>559</v>
-      </c>
-      <c r="C93" t="s">
-        <v>366</v>
-      </c>
-      <c r="D93" t="s">
-        <v>372</v>
-      </c>
-      <c r="E93" t="s">
-        <v>560</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J93" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10">
-      <c r="A94" t="s">
-        <v>561</v>
-      </c>
-      <c r="C94" t="s">
-        <v>375</v>
-      </c>
-      <c r="D94" t="s">
-        <v>376</v>
-      </c>
-      <c r="E94" t="s">
-        <v>562</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J94" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10">
-      <c r="A95" t="s">
-        <v>563</v>
-      </c>
-      <c r="C95" t="s">
-        <v>379</v>
-      </c>
-      <c r="D95" t="s">
-        <v>372</v>
-      </c>
-      <c r="E95" t="s">
-        <v>564</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J95" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10">
-      <c r="A96" t="s">
-        <v>565</v>
-      </c>
-      <c r="C96" t="s">
-        <v>382</v>
-      </c>
-      <c r="D96" t="s">
-        <v>367</v>
-      </c>
-      <c r="E96" t="s">
-        <v>566</v>
-      </c>
-      <c r="F96" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J96" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10">
-      <c r="A97" t="s">
-        <v>567</v>
-      </c>
-      <c r="C97" t="s">
-        <v>385</v>
-      </c>
-      <c r="D97" t="s">
-        <v>386</v>
-      </c>
-      <c r="E97" t="s">
-        <v>568</v>
-      </c>
-      <c r="F97" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J97" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10">
-      <c r="A98" t="s">
-        <v>569</v>
-      </c>
-      <c r="C98" t="s">
-        <v>366</v>
-      </c>
-      <c r="D98" t="s">
-        <v>367</v>
-      </c>
-      <c r="E98" t="s">
-        <v>570</v>
-      </c>
-      <c r="F98" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J98" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10">
-      <c r="A99" t="s">
-        <v>571</v>
-      </c>
-      <c r="C99" t="s">
-        <v>366</v>
-      </c>
-      <c r="D99" t="s">
-        <v>372</v>
-      </c>
-      <c r="E99" t="s">
-        <v>572</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J99" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10">
-      <c r="A100" t="s">
-        <v>573</v>
-      </c>
-      <c r="C100" t="s">
-        <v>375</v>
-      </c>
-      <c r="D100" t="s">
-        <v>376</v>
-      </c>
-      <c r="E100" t="s">
-        <v>574</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J100" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10">
-      <c r="A101" t="s">
-        <v>575</v>
-      </c>
-      <c r="C101" t="s">
-        <v>379</v>
-      </c>
-      <c r="D101" t="s">
-        <v>372</v>
-      </c>
-      <c r="E101" t="s">
-        <v>576</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J101" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10">
-      <c r="A102" t="s">
-        <v>577</v>
-      </c>
-      <c r="C102" t="s">
-        <v>382</v>
-      </c>
-      <c r="D102" t="s">
-        <v>367</v>
-      </c>
-      <c r="E102" t="s">
-        <v>578</v>
-      </c>
-      <c r="F102" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J102" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10">
-      <c r="A103" t="s">
-        <v>579</v>
-      </c>
-      <c r="C103" t="s">
-        <v>385</v>
-      </c>
-      <c r="D103" t="s">
-        <v>386</v>
-      </c>
-      <c r="E103" t="s">
-        <v>580</v>
-      </c>
-      <c r="F103" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J103" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10">
-      <c r="A104" t="s">
-        <v>581</v>
-      </c>
-      <c r="C104" t="s">
-        <v>366</v>
-      </c>
-      <c r="D104" t="s">
-        <v>367</v>
-      </c>
-      <c r="E104" t="s">
-        <v>582</v>
-      </c>
-      <c r="F104" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J104" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10">
-      <c r="A105" t="s">
-        <v>583</v>
-      </c>
-      <c r="C105" t="s">
-        <v>366</v>
-      </c>
-      <c r="D105" t="s">
-        <v>372</v>
-      </c>
-      <c r="E105" t="s">
-        <v>584</v>
-      </c>
-      <c r="F105" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J105" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10">
-      <c r="A106" t="s">
-        <v>585</v>
-      </c>
-      <c r="C106" t="s">
-        <v>375</v>
-      </c>
-      <c r="D106" t="s">
-        <v>376</v>
-      </c>
-      <c r="E106" t="s">
-        <v>586</v>
-      </c>
-      <c r="F106" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J106" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10">
-      <c r="A107" t="s">
-        <v>587</v>
-      </c>
-      <c r="C107" t="s">
-        <v>379</v>
-      </c>
-      <c r="D107" t="s">
-        <v>372</v>
-      </c>
-      <c r="E107" t="s">
-        <v>588</v>
-      </c>
-      <c r="F107" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J107" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10">
-      <c r="A108" t="s">
-        <v>589</v>
-      </c>
-      <c r="C108" t="s">
-        <v>382</v>
-      </c>
-      <c r="D108" t="s">
-        <v>367</v>
-      </c>
-      <c r="E108" t="s">
-        <v>590</v>
-      </c>
-      <c r="F108" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J108" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="109" spans="1:10">
-      <c r="A109" t="s">
-        <v>591</v>
-      </c>
-      <c r="C109" t="s">
-        <v>385</v>
-      </c>
-      <c r="D109" t="s">
-        <v>386</v>
-      </c>
-      <c r="E109" t="s">
-        <v>592</v>
-      </c>
-      <c r="F109" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J109" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="110" spans="1:10">
-      <c r="A110" t="s">
-        <v>593</v>
-      </c>
-      <c r="C110" t="s">
-        <v>366</v>
-      </c>
-      <c r="D110" t="s">
-        <v>367</v>
-      </c>
-      <c r="E110" t="s">
-        <v>594</v>
-      </c>
-      <c r="F110" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J110" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="111" spans="1:10">
-      <c r="A111" t="s">
-        <v>595</v>
-      </c>
-      <c r="C111" t="s">
-        <v>366</v>
-      </c>
-      <c r="D111" t="s">
-        <v>372</v>
-      </c>
-      <c r="E111" t="s">
-        <v>596</v>
-      </c>
-      <c r="F111" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J111" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="112" spans="1:10">
-      <c r="A112" t="s">
-        <v>597</v>
-      </c>
-      <c r="C112" t="s">
-        <v>375</v>
-      </c>
-      <c r="D112" t="s">
-        <v>376</v>
-      </c>
-      <c r="E112" t="s">
-        <v>598</v>
-      </c>
-      <c r="F112" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J112" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="113" spans="1:10">
-      <c r="A113" t="s">
-        <v>599</v>
-      </c>
-      <c r="C113" t="s">
-        <v>379</v>
-      </c>
-      <c r="D113" t="s">
-        <v>372</v>
-      </c>
-      <c r="E113" t="s">
-        <v>600</v>
-      </c>
-      <c r="F113" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J113" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="114" spans="1:10">
-      <c r="A114" t="s">
-        <v>601</v>
-      </c>
-      <c r="C114" t="s">
-        <v>382</v>
-      </c>
-      <c r="D114" t="s">
-        <v>367</v>
-      </c>
-      <c r="E114" t="s">
-        <v>602</v>
-      </c>
-      <c r="F114" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J114" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="115" spans="1:10">
-      <c r="A115" t="s">
-        <v>603</v>
-      </c>
-      <c r="C115" t="s">
-        <v>385</v>
-      </c>
-      <c r="D115" t="s">
-        <v>386</v>
-      </c>
-      <c r="E115" t="s">
-        <v>604</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="J115" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="116" spans="1:10">
-      <c r="A116" t="s">
-        <v>605</v>
-      </c>
-      <c r="C116" t="s">
-        <v>366</v>
-      </c>
-      <c r="D116" t="s">
-        <v>367</v>
-      </c>
-      <c r="E116" t="s">
-        <v>606</v>
-      </c>
-      <c r="F116" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J116" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10">
-      <c r="A117" t="s">
-        <v>607</v>
-      </c>
-      <c r="C117" t="s">
-        <v>366</v>
-      </c>
-      <c r="D117" t="s">
-        <v>372</v>
-      </c>
-      <c r="E117" t="s">
-        <v>608</v>
-      </c>
-      <c r="F117" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J117" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10">
-      <c r="A118" t="s">
-        <v>609</v>
-      </c>
-      <c r="C118" t="s">
-        <v>375</v>
-      </c>
-      <c r="D118" t="s">
-        <v>376</v>
-      </c>
-      <c r="E118" t="s">
-        <v>610</v>
-      </c>
-      <c r="F118" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J118" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10">
-      <c r="A119" t="s">
-        <v>611</v>
-      </c>
-      <c r="C119" t="s">
-        <v>379</v>
-      </c>
-      <c r="D119" t="s">
-        <v>372</v>
-      </c>
-      <c r="E119" t="s">
-        <v>612</v>
-      </c>
-      <c r="F119" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J119" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10">
-      <c r="A120" t="s">
-        <v>613</v>
-      </c>
-      <c r="C120" t="s">
-        <v>382</v>
-      </c>
-      <c r="D120" t="s">
-        <v>367</v>
-      </c>
-      <c r="E120" t="s">
-        <v>614</v>
-      </c>
-      <c r="F120" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J120" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10">
-      <c r="A121" t="s">
-        <v>615</v>
-      </c>
-      <c r="C121" t="s">
-        <v>385</v>
-      </c>
-      <c r="D121" t="s">
-        <v>386</v>
-      </c>
-      <c r="E121" t="s">
-        <v>616</v>
-      </c>
-      <c r="F121" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="J121" t="s">
         <v>370</v>
       </c>
     </row>
@@ -6790,102 +4291,6 @@
     <hyperlink ref="F23" r:id="rId22"/>
     <hyperlink ref="F24" r:id="rId23"/>
     <hyperlink ref="F25" r:id="rId24"/>
-    <hyperlink ref="F26" r:id="rId25"/>
-    <hyperlink ref="F27" r:id="rId26"/>
-    <hyperlink ref="F28" r:id="rId27"/>
-    <hyperlink ref="F29" r:id="rId28"/>
-    <hyperlink ref="F30" r:id="rId29"/>
-    <hyperlink ref="F31" r:id="rId30"/>
-    <hyperlink ref="F32" r:id="rId31"/>
-    <hyperlink ref="F33" r:id="rId32"/>
-    <hyperlink ref="F34" r:id="rId33"/>
-    <hyperlink ref="F35" r:id="rId34"/>
-    <hyperlink ref="F36" r:id="rId35"/>
-    <hyperlink ref="F37" r:id="rId36"/>
-    <hyperlink ref="F38" r:id="rId37"/>
-    <hyperlink ref="F39" r:id="rId38"/>
-    <hyperlink ref="F40" r:id="rId39"/>
-    <hyperlink ref="F41" r:id="rId40"/>
-    <hyperlink ref="F42" r:id="rId41"/>
-    <hyperlink ref="F43" r:id="rId42"/>
-    <hyperlink ref="F44" r:id="rId43"/>
-    <hyperlink ref="F45" r:id="rId44"/>
-    <hyperlink ref="F46" r:id="rId45"/>
-    <hyperlink ref="F47" r:id="rId46"/>
-    <hyperlink ref="F48" r:id="rId47"/>
-    <hyperlink ref="F49" r:id="rId48"/>
-    <hyperlink ref="F50" r:id="rId49"/>
-    <hyperlink ref="F51" r:id="rId50"/>
-    <hyperlink ref="F52" r:id="rId51"/>
-    <hyperlink ref="F53" r:id="rId52"/>
-    <hyperlink ref="F54" r:id="rId53"/>
-    <hyperlink ref="F55" r:id="rId54"/>
-    <hyperlink ref="F56" r:id="rId55"/>
-    <hyperlink ref="F57" r:id="rId56"/>
-    <hyperlink ref="F58" r:id="rId57"/>
-    <hyperlink ref="F59" r:id="rId58"/>
-    <hyperlink ref="F60" r:id="rId59"/>
-    <hyperlink ref="F61" r:id="rId60"/>
-    <hyperlink ref="F62" r:id="rId61"/>
-    <hyperlink ref="F63" r:id="rId62"/>
-    <hyperlink ref="F64" r:id="rId63"/>
-    <hyperlink ref="F65" r:id="rId64"/>
-    <hyperlink ref="F66" r:id="rId65"/>
-    <hyperlink ref="F67" r:id="rId66"/>
-    <hyperlink ref="F68" r:id="rId67"/>
-    <hyperlink ref="F69" r:id="rId68"/>
-    <hyperlink ref="F70" r:id="rId69"/>
-    <hyperlink ref="F71" r:id="rId70"/>
-    <hyperlink ref="F72" r:id="rId71"/>
-    <hyperlink ref="F73" r:id="rId72"/>
-    <hyperlink ref="F74" r:id="rId73"/>
-    <hyperlink ref="F75" r:id="rId74"/>
-    <hyperlink ref="F76" r:id="rId75"/>
-    <hyperlink ref="F77" r:id="rId76"/>
-    <hyperlink ref="F78" r:id="rId77"/>
-    <hyperlink ref="F79" r:id="rId78"/>
-    <hyperlink ref="F80" r:id="rId79"/>
-    <hyperlink ref="F81" r:id="rId80"/>
-    <hyperlink ref="F82" r:id="rId81"/>
-    <hyperlink ref="F83" r:id="rId82"/>
-    <hyperlink ref="F84" r:id="rId83"/>
-    <hyperlink ref="F85" r:id="rId84"/>
-    <hyperlink ref="F86" r:id="rId85"/>
-    <hyperlink ref="F87" r:id="rId86"/>
-    <hyperlink ref="F88" r:id="rId87"/>
-    <hyperlink ref="F89" r:id="rId88"/>
-    <hyperlink ref="F90" r:id="rId89"/>
-    <hyperlink ref="F91" r:id="rId90"/>
-    <hyperlink ref="F92" r:id="rId91"/>
-    <hyperlink ref="F93" r:id="rId92"/>
-    <hyperlink ref="F94" r:id="rId93"/>
-    <hyperlink ref="F95" r:id="rId94"/>
-    <hyperlink ref="F96" r:id="rId95"/>
-    <hyperlink ref="F97" r:id="rId96"/>
-    <hyperlink ref="F98" r:id="rId97"/>
-    <hyperlink ref="F99" r:id="rId98"/>
-    <hyperlink ref="F100" r:id="rId99"/>
-    <hyperlink ref="F101" r:id="rId100"/>
-    <hyperlink ref="F102" r:id="rId101"/>
-    <hyperlink ref="F103" r:id="rId102"/>
-    <hyperlink ref="F104" r:id="rId103"/>
-    <hyperlink ref="F105" r:id="rId104"/>
-    <hyperlink ref="F106" r:id="rId105"/>
-    <hyperlink ref="F107" r:id="rId106"/>
-    <hyperlink ref="F108" r:id="rId107"/>
-    <hyperlink ref="F109" r:id="rId108"/>
-    <hyperlink ref="F110" r:id="rId109"/>
-    <hyperlink ref="F111" r:id="rId110"/>
-    <hyperlink ref="F112" r:id="rId111"/>
-    <hyperlink ref="F113" r:id="rId112"/>
-    <hyperlink ref="F114" r:id="rId113"/>
-    <hyperlink ref="F115" r:id="rId114"/>
-    <hyperlink ref="F116" r:id="rId115"/>
-    <hyperlink ref="F117" r:id="rId116"/>
-    <hyperlink ref="F118" r:id="rId117"/>
-    <hyperlink ref="F119" r:id="rId118"/>
-    <hyperlink ref="F120" r:id="rId119"/>
-    <hyperlink ref="F121" r:id="rId120"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>